<commit_message>
some modifications are done
</commit_message>
<xml_diff>
--- a/mainAssignment/resources/movieDetails.xlsx
+++ b/mainAssignment/resources/movieDetails.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -433,11 +433,11 @@
   </sheetPr>
   <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5" outlineLevelCol="0"/>
   <cols>
     <col width="16.81640625" customWidth="1" min="1" max="1"/>
     <col width="15.08984375" customWidth="1" min="2" max="2"/>
@@ -706,13 +706,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5" outlineLevelCol="0"/>
   <cols>
     <col width="15.26953125" customWidth="1" min="1" max="1"/>
     <col width="15.1796875" customWidth="1" min="2" max="2"/>
@@ -751,81 +751,54 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>manikanth</t>
+          <t>steve</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>mani@dd.com</t>
+          <t>steve@123.com</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>987654321</t>
+          <t>1234567890</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>25</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>mani@123</t>
+          <t>steve@123</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>steve</t>
+          <t>mani</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>steve@123.com</t>
+          <t>mani@123.com</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>1234567890</t>
+          <t>987654321</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>25</t>
+          <t>20</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>steve@123</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>sai</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>sai12.com</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>12345</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>22</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>sai123</t>
+          <t>mani123</t>
         </is>
       </c>
     </row>

</xml_diff>